<commit_message>
working on crossplot & histogram
</commit_message>
<xml_diff>
--- a/Wi-CrossPlot.xlsx
+++ b/Wi-CrossPlot.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="78">
   <si>
     <t>Code</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t xml:space="preserve">         1.12.1</t>
+  </si>
+  <si>
+    <t>height-auto</t>
   </si>
 </sst>
 </file>
@@ -616,7 +619,7 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1013,6 +1016,9 @@
       <c r="J14" t="s">
         <v>12</v>
       </c>
+      <c r="L14" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
@@ -1038,6 +1044,9 @@
       <c r="J15" t="s">
         <v>12</v>
       </c>
+      <c r="L15" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
@@ -1063,8 +1072,11 @@
       <c r="J16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>70</v>
       </c>
@@ -1088,8 +1100,11 @@
       <c r="J17" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>71</v>
       </c>
@@ -1113,8 +1128,11 @@
       <c r="J18" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>72</v>
       </c>
@@ -1138,8 +1156,11 @@
       <c r="J19" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>73</v>
       </c>
@@ -1163,8 +1184,11 @@
       <c r="J20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>74</v>
       </c>
@@ -1188,8 +1212,11 @@
       <c r="J21" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>75</v>
       </c>
@@ -1214,7 +1241,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>76</v>
       </c>
@@ -1238,8 +1265,11 @@
       <c r="J23" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D24" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1249,7 +1279,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D25" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1259,7 +1289,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D26" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1269,7 +1299,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D27" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1279,7 +1309,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D28" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1289,7 +1319,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D29" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1299,7 +1329,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D30" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1309,7 +1339,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D31" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1319,7 +1349,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D32" t="str">
         <f t="shared" si="4"/>
         <v/>

</xml_diff>